<commit_message>
New Test Added for Auto programming
</commit_message>
<xml_diff>
--- a/Data Files/Complete_Questionaire_Comments.xlsx
+++ b/Data Files/Complete_Questionaire_Comments.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4D2A34-D16E-44BB-A9E7-1730D379D15B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810C69D7-7987-4156-B562-95D774ADF210}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Verifications</t>
   </si>
@@ -29,11 +29,38 @@
   </si>
   <si>
     <t>Having reviewed the appeal submission documents, do you agree that the information provided accurately reflects the original application?</t>
+  </si>
+  <si>
+    <t>Upload any relevant adopted development plan policies</t>
+  </si>
+  <si>
+    <t>Questionnaire received</t>
+  </si>
+  <si>
+    <t>^Questionnaire reference number.*</t>
+  </si>
+  <si>
+    <t>Final comments received</t>
+  </si>
+  <si>
+    <t>^Final comments reference number.*</t>
+  </si>
+  <si>
+    <t>^Statement reference number.*</t>
+  </si>
+  <si>
+    <t>Statement received</t>
+  </si>
+  <si>
+    <t>Comments received</t>
+  </si>
+  <si>
+    <t>^Comments reference number.*</t>
   </si>
   <si>
     <t>Appeal information
 Appeal procedure
-Local Policy
+Local policies
 Emerging policies
 Five year housing land supply
 Conditions and obligations
@@ -41,36 +68,48 @@
 Monuments and listed buildings
 Environmental screening
 The planning application
-Notifications
-Upload other files
+Notifications and correspondence
+Bulk file upload
 Confirmation</t>
   </si>
   <si>
-    <t>Upload any relevant adopted development plan policies</t>
-  </si>
-  <si>
-    <t>Questionnaire received</t>
-  </si>
-  <si>
-    <t>^Questionnaire reference number.*</t>
-  </si>
-  <si>
-    <t>Final comments received</t>
-  </si>
-  <si>
-    <t>^Final comments reference number.*</t>
-  </si>
-  <si>
-    <t>^Statement reference number.*</t>
-  </si>
-  <si>
-    <t>Statement received</t>
-  </si>
-  <si>
-    <t>Comments received</t>
-  </si>
-  <si>
-    <t>^Comments reference number.*</t>
+    <t>Automated_Test</t>
+  </si>
+  <si>
+    <t>OPEN FOR LPA STATEMENT AND INTERESTED PARTY REPRESENTATIONS</t>
+  </si>
+  <si>
+    <t>Appeal information
+Appeal procedure
+Local policies
+Emerging policies
+Conditions and obligations
+Conservation areas
+Monuments and listed buildings
+Environmental screening
+The planning application
+Notifications and correspondence
+Upload the plans
+Bulk file upload
+Additional Information
+Confirmation</t>
+  </si>
+  <si>
+    <t>Appeal information
+Appeal follows
+Appeal procedure
+Local policies
+Emerging policies
+Conditions and obligations
+Conservation areas
+Monuments and listed buildings
+Environmental screening
+The planning application
+Notifications and correspondence
+Upload the plans
+Special control
+Bulk file upload
+Confirmation</t>
   </si>
 </sst>
 </file>
@@ -391,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -419,62 +458,82 @@
     </row>
     <row r="4" spans="1:1" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="203" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Test added for Backstage and disabled Appeal Summary verification
</commit_message>
<xml_diff>
--- a/Data Files/Complete_Questionaire_Comments.xlsx
+++ b/Data Files/Complete_Questionaire_Comments.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810C69D7-7987-4156-B562-95D774ADF210}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E7D6AD-69A3-402E-8DA9-030E4BDA774C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Verifications</t>
   </si>
@@ -110,6 +110,12 @@
 Special control
 Bulk file upload
 Confirmation</t>
+  </si>
+  <si>
+    <t>Appellant statement received</t>
+  </si>
+  <si>
+    <t>Appellant statement reference number</t>
   </si>
 </sst>
 </file>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,6 +542,16 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
New script added for Cost Application portal screen.
</commit_message>
<xml_diff>
--- a/Data Files/Complete_Questionaire_Comments.xlsx
+++ b/Data Files/Complete_Questionaire_Comments.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E7D6AD-69A3-402E-8DA9-030E4BDA774C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27FEE56-9976-4DB1-9ECA-7E4F13B574FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Verifications</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Appellant statement reference number</t>
+  </si>
+  <si>
+    <t>Cost response received</t>
+  </si>
+  <si>
+    <t>Cost response reference number</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,6 +558,16 @@
         <v>18</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated HAS questionnaire script and data file.
</commit_message>
<xml_diff>
--- a/Data Files/Complete_Questionaire_Comments.xlsx
+++ b/Data Files/Complete_Questionaire_Comments.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27FEE56-9976-4DB1-9ECA-7E4F13B574FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CC5B68-A0EE-46B1-B41E-30C3C47EB747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,22 +80,6 @@
   </si>
   <si>
     <t>Appeal information
-Appeal procedure
-Local policies
-Emerging policies
-Conditions and obligations
-Conservation areas
-Monuments and listed buildings
-Environmental screening
-The planning application
-Notifications and correspondence
-Upload the plans
-Bulk file upload
-Additional Information
-Confirmation</t>
-  </si>
-  <si>
-    <t>Appeal information
 Appeal follows
 Appeal procedure
 Local policies
@@ -122,6 +106,20 @@
   </si>
   <si>
     <t>Cost response reference number</t>
+  </si>
+  <si>
+    <t>Appeal information
+Site accessibility
+Conservation areas
+Monuments and listed buildings
+Plans
+Planning Officer's Report
+Interested Parties and Consultees
+Interested Parties and Consultee Comments
+Local policy
+Suggested Conditions
+Additional Information
+Confirmation</t>
   </si>
 </sst>
 </file>
@@ -444,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,9 +526,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="203" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="174" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
@@ -545,27 +543,27 @@
     </row>
     <row r="19" spans="1:1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes applied to HAS questionnaire script.
</commit_message>
<xml_diff>
--- a/Data Files/Complete_Questionaire_Comments.xlsx
+++ b/Data Files/Complete_Questionaire_Comments.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CC5B68-A0EE-46B1-B41E-30C3C47EB747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D130CCA-88FF-453C-A9F2-2CFBA5E7B4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,6 +115,7 @@
 Plans
 Planning Officer's Report
 Interested Parties and Consultees
+Notification letter
 Interested Parties and Consultee Comments
 Local policy
 Suggested Conditions
@@ -526,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>